<commit_message>
fixed a problem with Boot mode of the main board. Added micro switch with pull-up resistor for gpio8. Fixed pinout on BME280 sensor board for compatibility with Grove sensors.
</commit_message>
<xml_diff>
--- a/Altruist/PCB/Mainboard/BOM_Altruist.xlsx
+++ b/Altruist/PCB/Mainboard/BOM_Altruist.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_Altruist_core_ESP32C3mini_A" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Altruist_PCB_Altruist_2025-" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="329">
   <si>
     <t>No.</t>
   </si>
@@ -82,10 +82,10 @@
     <t>CONN-TH_2P-P5.00_CPC3703CTR</t>
   </si>
   <si>
-    <t>0.1074</t>
-  </si>
-  <si>
-    <t>1124</t>
+    <t>0.105</t>
+  </si>
+  <si>
+    <t>3714</t>
   </si>
   <si>
     <t>2</t>
@@ -109,7 +109,7 @@
     <t>0.0377</t>
   </si>
   <si>
-    <t>141799</t>
+    <t>60915</t>
   </si>
   <si>
     <t>3</t>
@@ -136,7 +136,7 @@
     <t>0.0899</t>
   </si>
   <si>
-    <t>133718</t>
+    <t>244832</t>
   </si>
   <si>
     <t>4</t>
@@ -160,10 +160,10 @@
     <t>C0603</t>
   </si>
   <si>
-    <t>0.027</t>
-  </si>
-  <si>
-    <t>957108</t>
+    <t>0.0305</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>5</t>
@@ -187,544 +187,547 @@
     <t>C0402</t>
   </si>
   <si>
+    <t>0.0019</t>
+  </si>
+  <si>
+    <t>282795</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>UV2G3R3M0810</t>
+  </si>
+  <si>
+    <t>C6,C7</t>
+  </si>
+  <si>
+    <t>3.3uF</t>
+  </si>
+  <si>
+    <t>HONOR(荣誉)</t>
+  </si>
+  <si>
+    <t>C98554</t>
+  </si>
+  <si>
+    <t>CAP-SMD_BD8.0-L8.3-W8.3-FD</t>
+  </si>
+  <si>
+    <t>0.0876</t>
+  </si>
+  <si>
+    <t>2282</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1206B103K102CT_C77498</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>1206B103K102CT</t>
+  </si>
+  <si>
+    <t>C77498</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>0.0103</t>
+  </si>
+  <si>
+    <t>25083</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>CL21A225KBQNNNE</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>SAMSUNG(三星)</t>
+  </si>
+  <si>
+    <t>C377773</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>0.0148</t>
+  </si>
+  <si>
+    <t>1113408</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>TAJE687K006RNJ</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>680uF</t>
+  </si>
+  <si>
+    <t>KyoceraAVX</t>
+  </si>
+  <si>
+    <t>C308811</t>
+  </si>
+  <si>
+    <t>CAP-SMD_L7.3-W4.3</t>
+  </si>
+  <si>
+    <t>1.179</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>ZX-SH1.0-4PWT</t>
+  </si>
+  <si>
+    <t>CN5</t>
+  </si>
+  <si>
+    <t>Megastar(兆星)</t>
+  </si>
+  <si>
+    <t>C7430446</t>
+  </si>
+  <si>
+    <t>CONN-SMD_4P-P1.00_MEGASTAR_ZX-SH1.0-4PWT</t>
+  </si>
+  <si>
+    <t>0.0771</t>
+  </si>
+  <si>
+    <t>820</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>LESD5D5.0CT1G</t>
+  </si>
+  <si>
+    <t>D1,D5,D6,D7</t>
+  </si>
+  <si>
+    <t>LRC(乐山无线电)</t>
+  </si>
+  <si>
+    <t>C383211</t>
+  </si>
+  <si>
+    <t>SOD-523_L1.2-W0.8-LS1.6-BI</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>40828</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1N5819WS_C191023</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>1N5819WS</t>
+  </si>
+  <si>
+    <t>Hottech(合科泰)</t>
+  </si>
+  <si>
+    <t>C191023</t>
+  </si>
+  <si>
+    <t>SOD-323_L1.8-W1.3-LS2.5-RD</t>
+  </si>
+  <si>
+    <t>0.0095</t>
+  </si>
+  <si>
+    <t>1584233</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>MB10F_C306850</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>MB10F</t>
+  </si>
+  <si>
+    <t>BORN(伯恩半导体)</t>
+  </si>
+  <si>
+    <t>C306850</t>
+  </si>
+  <si>
+    <t>MBF_L4.8-W3.9-P2.50-LS6.7-BL</t>
+  </si>
+  <si>
+    <t>0.0264</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>ES1J_C115404</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>ES1J</t>
+  </si>
+  <si>
+    <t>晶导微电子</t>
+  </si>
+  <si>
+    <t>C115404</t>
+  </si>
+  <si>
+    <t>SMA_L4.3-W2.6-LS5.2-RD</t>
+  </si>
+  <si>
+    <t>0.0136</t>
+  </si>
+  <si>
+    <t>1806</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>JFC2410-1200FS</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>JDTfuse(集电通)</t>
+  </si>
+  <si>
+    <t>C136365</t>
+  </si>
+  <si>
+    <t>F2410</t>
+  </si>
+  <si>
+    <t>0.0708</t>
+  </si>
+  <si>
+    <t>7775</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>YNR6045-681M</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>680uH</t>
+  </si>
+  <si>
+    <t>YJYCOIN(益嘉源)</t>
+  </si>
+  <si>
+    <t>C497844</t>
+  </si>
+  <si>
+    <t>IND-SMD_L6.0-W6.0</t>
+  </si>
+  <si>
+    <t>0.0726</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>YNR8040-471M</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>470uH</t>
+  </si>
+  <si>
+    <t>C341087</t>
+  </si>
+  <si>
+    <t>IND-SMD_L8.0-W8.0</t>
+  </si>
+  <si>
+    <t>0.1254</t>
+  </si>
+  <si>
+    <t>1831</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>X8821WR-05S-N0SN</t>
+  </si>
+  <si>
+    <t>PMSensor</t>
+  </si>
+  <si>
+    <t>XKBConnectivity(中国星坤)</t>
+  </si>
+  <si>
+    <t>C388742</t>
+  </si>
+  <si>
+    <t>CONN-TH_5P-P2.50_X8821WR-05S-N0SN</t>
+  </si>
+  <si>
+    <t>0.0392</t>
+  </si>
+  <si>
+    <t>1252</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3V_C5120796</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3V</t>
+  </si>
+  <si>
+    <t>MSKSEMI(美森科)</t>
+  </si>
+  <si>
+    <t>C5120796</t>
+  </si>
+  <si>
+    <t>SOT-89-3_L4.5-W2.5-P1.50-LS4.2-BR</t>
+  </si>
+  <si>
+    <t>0.0405</t>
+  </si>
+  <si>
+    <t>90929</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>AC1206FR-071M5L</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>1.5MΩ</t>
+  </si>
+  <si>
+    <t>YAGEO(国巨)</t>
+  </si>
+  <si>
+    <t>C229411</t>
+  </si>
+  <si>
+    <t>R1206</t>
+  </si>
+  <si>
+    <t>0.0144</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>0805W8F3602T5E</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>36kΩ</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(厚声)</t>
+  </si>
+  <si>
+    <t>C4360</t>
+  </si>
+  <si>
+    <t>R0805</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>77857</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>0805W8F1002T5E</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>C17414</t>
+  </si>
+  <si>
+    <t>0.0017</t>
+  </si>
+  <si>
+    <t>13777142</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>07D471K68RV0149</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>KNSCHA(科尼盛)</t>
+  </si>
+  <si>
+    <t>C2836432</t>
+  </si>
+  <si>
+    <t>RES-SMD_L8.2-W6.3</t>
+  </si>
+  <si>
+    <t>0.0695</t>
+  </si>
+  <si>
+    <t>14359</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>R6,R11,R12,R19</t>
+  </si>
+  <si>
+    <t>C60490</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>0.0006</t>
+  </si>
+  <si>
+    <t>6790753</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>0805W8F820LT5E</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>820mΩ</t>
+  </si>
+  <si>
+    <t>C25267</t>
+  </si>
+  <si>
+    <t>0.0032</t>
+  </si>
+  <si>
+    <t>5909</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>0805W8J0000T5E</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>0Ω</t>
+  </si>
+  <si>
+    <t>C25275</t>
+  </si>
+  <si>
     <t>0.0016</t>
   </si>
   <si>
-    <t>1657159</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>UV2G3R3M0810</t>
-  </si>
-  <si>
-    <t>C6,C7</t>
-  </si>
-  <si>
-    <t>3.3uF</t>
-  </si>
-  <si>
-    <t>HONOR(荣誉)</t>
-  </si>
-  <si>
-    <t>C98554</t>
-  </si>
-  <si>
-    <t>CAP-SMD_BD8.0-L8.3-W8.3-FD</t>
-  </si>
-  <si>
-    <t>0.1091</t>
-  </si>
-  <si>
-    <t>2882</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1206B103K102CT_C77498</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>1206B103K102CT</t>
-  </si>
-  <si>
-    <t>C77498</t>
-  </si>
-  <si>
-    <t>C1206</t>
-  </si>
-  <si>
-    <t>0.0085</t>
-  </si>
-  <si>
-    <t>71834</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>CL21A225KBQNNNE</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>SAMSUNG(三星)</t>
-  </si>
-  <si>
-    <t>C377773</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
-    <t>0.0132</t>
-  </si>
-  <si>
-    <t>327200</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>TAJE687K006RNJ</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>680uF</t>
-  </si>
-  <si>
-    <t>KyoceraAVX</t>
-  </si>
-  <si>
-    <t>C308811</t>
-  </si>
-  <si>
-    <t>CAP-SMD_L7.3-W4.3</t>
-  </si>
-  <si>
-    <t>1.179</t>
-  </si>
-  <si>
-    <t>838</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>ZX-SH1.0-4PWT</t>
-  </si>
-  <si>
-    <t>CN5</t>
-  </si>
-  <si>
-    <t>Megastar(兆星)</t>
-  </si>
-  <si>
-    <t>C7430446</t>
-  </si>
-  <si>
-    <t>CONN-SMD_4P-P1.00_MEGASTAR_ZX-SH1.0-4PWT</t>
-  </si>
-  <si>
-    <t>0.0683</t>
-  </si>
-  <si>
-    <t>22026</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>LESD5D5.0CT1G</t>
-  </si>
-  <si>
-    <t>D1,D5,D6,D7</t>
-  </si>
-  <si>
-    <t>LRC(乐山无线电)</t>
-  </si>
-  <si>
-    <t>C383211</t>
-  </si>
-  <si>
-    <t>SOD-523_L1.2-W0.8-LS1.6-BI</t>
-  </si>
-  <si>
-    <t>0.0185</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>1N5819WS_C191023</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>1N5819WS</t>
-  </si>
-  <si>
-    <t>Hottech(合科泰)</t>
-  </si>
-  <si>
-    <t>C191023</t>
-  </si>
-  <si>
-    <t>SOD-323_L1.8-W1.3-LS2.5-RD</t>
-  </si>
-  <si>
-    <t>0.0079</t>
-  </si>
-  <si>
-    <t>744081</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>MB10F_C306850</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>MB10F</t>
-  </si>
-  <si>
-    <t>BORN(伯恩半导体)</t>
-  </si>
-  <si>
-    <t>C306850</t>
-  </si>
-  <si>
-    <t>MBF_L4.8-W3.9-P2.50-LS6.7-BL</t>
-  </si>
-  <si>
-    <t>0.0242</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>ES1J_C115404</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>ES1J</t>
-  </si>
-  <si>
-    <t>晶导微电子</t>
-  </si>
-  <si>
-    <t>C115404</t>
-  </si>
-  <si>
-    <t>SMA_L4.3-W2.6-LS5.2-RD</t>
-  </si>
-  <si>
-    <t>0.0123</t>
-  </si>
-  <si>
-    <t>17552</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>JFC2410-1200FS</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>JDTfuse(集电通)</t>
-  </si>
-  <si>
-    <t>C136365</t>
-  </si>
-  <si>
-    <t>F2410</t>
-  </si>
-  <si>
-    <t>0.0653</t>
-  </si>
-  <si>
-    <t>1118</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>YNR6045-681M</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>680uH</t>
-  </si>
-  <si>
-    <t>YJYCOIN(益嘉源)</t>
-  </si>
-  <si>
-    <t>C497844</t>
-  </si>
-  <si>
-    <t>IND-SMD_L6.0-W6.0</t>
-  </si>
-  <si>
-    <t>0.0638</t>
-  </si>
-  <si>
-    <t>1414</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>YNR8040-471M</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>470uH</t>
-  </si>
-  <si>
-    <t>C341087</t>
-  </si>
-  <si>
-    <t>IND-SMD_L8.0-W8.0</t>
-  </si>
-  <si>
-    <t>0.1104</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>X8821WR-05S-N0SN</t>
-  </si>
-  <si>
-    <t>PMSensor</t>
-  </si>
-  <si>
-    <t>XKBConnectivity(中国星坤)</t>
-  </si>
-  <si>
-    <t>C388742</t>
-  </si>
-  <si>
-    <t>CONN-TH_5P-P2.50_X8821WR-05S-N0SN</t>
-  </si>
-  <si>
-    <t>0.0363</t>
-  </si>
-  <si>
-    <t>7167</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>AMS1117-3.3V_C5120796</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>AMS1117-3.3V</t>
-  </si>
-  <si>
-    <t>MSKSEMI(美森科)</t>
-  </si>
-  <si>
-    <t>C5120796</t>
-  </si>
-  <si>
-    <t>SOT-89-3_L4.5-W2.5-P1.50-LS4.2-BR</t>
-  </si>
-  <si>
-    <t>0.0372</t>
-  </si>
-  <si>
-    <t>169625</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>AC1206FR-071M5L</t>
-  </si>
-  <si>
-    <t>R1,R2</t>
-  </si>
-  <si>
-    <t>1.5MΩ</t>
-  </si>
-  <si>
-    <t>YAGEO(国巨)</t>
-  </si>
-  <si>
-    <t>C229411</t>
-  </si>
-  <si>
-    <t>R1206</t>
-  </si>
-  <si>
-    <t>0.0128</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>0805W8F3602T5E</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>36kΩ</t>
-  </si>
-  <si>
-    <t>UNI-ROYAL(厚声)</t>
-  </si>
-  <si>
-    <t>C4360</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>0.0018</t>
-  </si>
-  <si>
-    <t>167731</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>0805W8F1002T5E</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
-    <t>C17414</t>
-  </si>
-  <si>
-    <t>9165564</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>07D471K68RV0149</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>KNSCHA(科尼盛)</t>
-  </si>
-  <si>
-    <t>C2836432</t>
-  </si>
-  <si>
-    <t>RES-SMD_L8.2-W6.3</t>
-  </si>
-  <si>
-    <t>0.0641</t>
-  </si>
-  <si>
-    <t>2428</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>R6,R11,R12</t>
-  </si>
-  <si>
-    <t>C60490</t>
-  </si>
-  <si>
-    <t>R0402</t>
+    <t>27</t>
+  </si>
+  <si>
+    <t>0402WGF5101TCE</t>
+  </si>
+  <si>
+    <t>R9,R10</t>
+  </si>
+  <si>
+    <t>5.1kΩ</t>
+  </si>
+  <si>
+    <t>C25905</t>
   </si>
   <si>
     <t>0.0005</t>
   </si>
   <si>
-    <t>6790566</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>0805W8F820LT5E</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>820mΩ</t>
-  </si>
-  <si>
-    <t>C25267</t>
-  </si>
-  <si>
-    <t>0.0033</t>
-  </si>
-  <si>
-    <t>5494</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>0805W8J0000T5E</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>0Ω</t>
-  </si>
-  <si>
-    <t>C25275</t>
-  </si>
-  <si>
-    <t>0.0014</t>
-  </si>
-  <si>
-    <t>225223</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>0402WGF5101TCE</t>
-  </si>
-  <si>
-    <t>R9,R10</t>
-  </si>
-  <si>
-    <t>5.1kΩ</t>
-  </si>
-  <si>
-    <t>C25905</t>
-  </si>
-  <si>
-    <t>4547772</t>
+    <t>2811828</t>
   </si>
   <si>
     <t>28</t>
@@ -742,7 +745,7 @@
     <t>C25092</t>
   </si>
   <si>
-    <t>2636260</t>
+    <t>3437242</t>
   </si>
   <si>
     <t>29</t>
@@ -763,10 +766,10 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>0.0009</t>
-  </si>
-  <si>
-    <t>16727911</t>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>23507784</t>
   </si>
   <si>
     <t>10K</t>
@@ -784,10 +787,10 @@
     <t>C23179</t>
   </si>
   <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>1968382</t>
+    <t>0.0011</t>
+  </si>
+  <si>
+    <t>2052918</t>
   </si>
   <si>
     <t>470</t>
@@ -805,7 +808,7 @@
     <t>C23162</t>
   </si>
   <si>
-    <t>4477115</t>
+    <t>5466286</t>
   </si>
   <si>
     <t>4.7kΩ</t>
@@ -829,10 +832,10 @@
     <t>CONN-TH_XH-4AW</t>
   </si>
   <si>
-    <t>0.0209</t>
-  </si>
-  <si>
-    <t>15920</t>
+    <t>0.0236</t>
+  </si>
+  <si>
+    <t>16268</t>
   </si>
   <si>
     <t>XH-4AW_C2908613</t>
@@ -856,10 +859,7 @@
     <t>CONN-SMD_HY2.0-4P</t>
   </si>
   <si>
-    <t>0.0609</t>
-  </si>
-  <si>
-    <t>405</t>
+    <t>0.0687</t>
   </si>
   <si>
     <t>HY2.0-4P-C146060</t>
@@ -868,6 +868,30 @@
     <t>34</t>
   </si>
   <si>
+    <t>DHN-02-V-T/R</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>圜达</t>
+  </si>
+  <si>
+    <t>C224995</t>
+  </si>
+  <si>
+    <t>SW-SMD_4P-L3.8-W4.5-P1.27-LS6.7</t>
+  </si>
+  <si>
+    <t>0.7785</t>
+  </si>
+  <si>
+    <t>3999</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>ESP32-C3-MINI-1-N4</t>
   </si>
   <si>
@@ -886,10 +910,10 @@
     <t>2.6385</t>
   </si>
   <si>
-    <t>570</t>
-  </si>
-  <si>
-    <t>35</t>
+    <t>7742</t>
+  </si>
+  <si>
+    <t>36</t>
   </si>
   <si>
     <t>SY50282FAC</t>
@@ -907,13 +931,13 @@
     <t>SOIC-8_L4.9-W3.9-P1.27-LS6.0-BL</t>
   </si>
   <si>
-    <t>0.2454</t>
-  </si>
-  <si>
-    <t>969</t>
-  </si>
-  <si>
-    <t>36</t>
+    <t>0.2798</t>
+  </si>
+  <si>
+    <t>824</t>
+  </si>
+  <si>
+    <t>37</t>
   </si>
   <si>
     <t>XY-ZH1.5-5A21</t>
@@ -931,10 +955,7 @@
     <t>CONN-TH_ZH1.5-5AW_C2829750</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>TYPE-C 16P QTWT</t>
@@ -952,13 +973,13 @@
     <t>USB-TYPE-C-SMD_TYPE-C-16P-QTWT</t>
   </si>
   <si>
-    <t>0.0704</t>
-  </si>
-  <si>
-    <t>10298</t>
-  </si>
-  <si>
-    <t>38</t>
+    <t>0.0779</t>
+  </si>
+  <si>
+    <t>18167</t>
+  </si>
+  <si>
+    <t>39</t>
   </si>
   <si>
     <t>19-217/GHC-YR1S2/3T</t>
@@ -976,10 +997,7 @@
     <t>LED0603-R-RD</t>
   </si>
   <si>
-    <t>0.0368</t>
-  </si>
-  <si>
-    <t>9911</t>
+    <t>0.041</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -1917,7 +1935,7 @@
         <v>110</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1931,96 +1949,96 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>118</v>
+      </c>
+      <c r="K13" t="s">
+        <v>119</v>
+      </c>
+      <c r="L13" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" t="s">
         <v>115</v>
-      </c>
-      <c r="H13" t="s">
-        <v>116</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s">
-        <v>117</v>
-      </c>
-      <c r="K13" t="s">
-        <v>118</v>
-      </c>
-      <c r="L13" t="s">
-        <v>119</v>
-      </c>
-      <c r="M13" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" t="s">
         <v>124</v>
-      </c>
-      <c r="H14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" t="s">
-        <v>126</v>
-      </c>
-      <c r="K14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L14" t="s">
-        <v>128</v>
-      </c>
-      <c r="M14" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" t="s">
-        <v>18</v>
-      </c>
-      <c r="O14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2340,7 +2358,7 @@
         <v>187</v>
       </c>
       <c r="L21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M21" t="s">
         <v>18</v>
@@ -2431,10 +2449,10 @@
         <v>194</v>
       </c>
       <c r="K23" t="s">
-        <v>58</v>
+        <v>202</v>
       </c>
       <c r="L23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M23" t="s">
         <v>18</v>
@@ -2448,40 +2466,40 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D24" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
         <v>205</v>
       </c>
-      <c r="E24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" t="s">
-        <v>204</v>
-      </c>
       <c r="G24" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I24" t="s">
         <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K24" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M24" t="s">
         <v>18</v>
@@ -2490,45 +2508,45 @@
         <v>18</v>
       </c>
       <c r="O24" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E25" t="s">
         <v>200</v>
       </c>
       <c r="F25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G25" t="s">
         <v>184</v>
       </c>
       <c r="H25" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I25" t="s">
         <v>21</v>
       </c>
       <c r="J25" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K25" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L25" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="M25" t="s">
         <v>18</v>
@@ -2542,28 +2560,28 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D26" t="s">
+        <v>221</v>
+      </c>
+      <c r="E26" t="s">
+        <v>222</v>
+      </c>
+      <c r="F26" t="s">
         <v>220</v>
-      </c>
-      <c r="E26" t="s">
-        <v>221</v>
-      </c>
-      <c r="F26" t="s">
-        <v>219</v>
       </c>
       <c r="G26" t="s">
         <v>192</v>
       </c>
       <c r="H26" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I26" t="s">
         <v>21</v>
@@ -2572,10 +2590,10 @@
         <v>194</v>
       </c>
       <c r="K26" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L26" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M26" t="s">
         <v>18</v>
@@ -2584,33 +2602,33 @@
         <v>18</v>
       </c>
       <c r="O26" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D27" t="s">
+        <v>228</v>
+      </c>
+      <c r="E27" t="s">
+        <v>229</v>
+      </c>
+      <c r="F27" t="s">
         <v>227</v>
-      </c>
-      <c r="E27" t="s">
-        <v>228</v>
-      </c>
-      <c r="F27" t="s">
-        <v>226</v>
       </c>
       <c r="G27" t="s">
         <v>192</v>
       </c>
       <c r="H27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I27" t="s">
         <v>21</v>
@@ -2619,10 +2637,10 @@
         <v>194</v>
       </c>
       <c r="K27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L27" t="s">
-        <v>231</v>
+        <v>112</v>
       </c>
       <c r="M27" t="s">
         <v>18</v>
@@ -2631,7 +2649,7 @@
         <v>18</v>
       </c>
       <c r="O27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2663,13 +2681,13 @@
         <v>21</v>
       </c>
       <c r="J28" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K28" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="L28" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M28" t="s">
         <v>18</v>
@@ -2683,87 +2701,87 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D29" t="s">
+        <v>241</v>
+      </c>
+      <c r="E29" t="s">
+        <v>242</v>
+      </c>
+      <c r="F29" t="s">
         <v>240</v>
-      </c>
-      <c r="E29" t="s">
-        <v>241</v>
-      </c>
-      <c r="F29" t="s">
-        <v>239</v>
       </c>
       <c r="G29" t="s">
         <v>192</v>
       </c>
       <c r="H29" t="s">
+        <v>243</v>
+      </c>
+      <c r="I29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" t="s">
+        <v>216</v>
+      </c>
+      <c r="K29" t="s">
+        <v>237</v>
+      </c>
+      <c r="L29" t="s">
+        <v>244</v>
+      </c>
+      <c r="M29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O29" t="s">
         <v>242</v>
-      </c>
-      <c r="I29" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" t="s">
-        <v>215</v>
-      </c>
-      <c r="K29" t="s">
-        <v>216</v>
-      </c>
-      <c r="L29" t="s">
-        <v>243</v>
-      </c>
-      <c r="M29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N29" t="s">
-        <v>18</v>
-      </c>
-      <c r="O29" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D30" t="s">
+        <v>247</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
         <v>246</v>
       </c>
-      <c r="E30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" t="s">
-        <v>245</v>
-      </c>
       <c r="G30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I30" t="s">
         <v>21</v>
       </c>
       <c r="J30" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K30" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M30" t="s">
         <v>18</v>
@@ -2772,45 +2790,45 @@
         <v>18</v>
       </c>
       <c r="O30" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D31" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
         <v>255</v>
       </c>
-      <c r="E31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" t="s">
-        <v>254</v>
-      </c>
       <c r="G31" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H31" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I31" t="s">
         <v>21</v>
       </c>
       <c r="J31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K31" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L31" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M31" t="s">
         <v>18</v>
@@ -2819,45 +2837,45 @@
         <v>18</v>
       </c>
       <c r="O31" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D32" t="s">
+        <v>263</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
         <v>262</v>
       </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" t="s">
-        <v>261</v>
-      </c>
       <c r="G32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H32" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I32" t="s">
         <v>21</v>
       </c>
       <c r="J32" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="K32" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L32" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M32" t="s">
         <v>18</v>
@@ -2866,45 +2884,45 @@
         <v>18</v>
       </c>
       <c r="O32" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D33" t="s">
+        <v>269</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
         <v>268</v>
       </c>
-      <c r="E33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" t="s">
-        <v>267</v>
-      </c>
       <c r="G33" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H33" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I33" t="s">
         <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K33" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L33" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M33" t="s">
         <v>18</v>
@@ -2913,45 +2931,45 @@
         <v>18</v>
       </c>
       <c r="O33" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D34" t="s">
+        <v>278</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
         <v>277</v>
       </c>
-      <c r="E34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" t="s">
-        <v>276</v>
-      </c>
       <c r="G34" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H34" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I34" t="s">
         <v>21</v>
       </c>
       <c r="J34" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="K34" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="L34" t="s">
-        <v>282</v>
+        <v>42</v>
       </c>
       <c r="M34" t="s">
         <v>18</v>
@@ -3089,10 +3107,10 @@
         <v>305</v>
       </c>
       <c r="K37" t="s">
-        <v>18</v>
+        <v>306</v>
       </c>
       <c r="L37" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M37" t="s">
         <v>18</v>
@@ -3106,40 +3124,40 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D38" t="s">
+        <v>310</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
         <v>309</v>
       </c>
-      <c r="E38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" t="s">
-        <v>308</v>
-      </c>
       <c r="G38" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H38" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="I38" t="s">
         <v>21</v>
       </c>
       <c r="J38" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K38" t="s">
-        <v>313</v>
+        <v>18</v>
       </c>
       <c r="L38" t="s">
-        <v>314</v>
+        <v>50</v>
       </c>
       <c r="M38" t="s">
         <v>18</v>
@@ -3148,58 +3166,105 @@
         <v>18</v>
       </c>
       <c r="O38" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>314</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>315</v>
       </c>
-      <c r="B39">
+      <c r="D39" t="s">
+        <v>316</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>315</v>
+      </c>
+      <c r="G39" t="s">
+        <v>317</v>
+      </c>
+      <c r="H39" t="s">
+        <v>318</v>
+      </c>
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>319</v>
+      </c>
+      <c r="K39" t="s">
+        <v>320</v>
+      </c>
+      <c r="L39" t="s">
+        <v>321</v>
+      </c>
+      <c r="M39" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" t="s">
+        <v>18</v>
+      </c>
+      <c r="O39" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>322</v>
+      </c>
+      <c r="B40">
         <v>2</v>
       </c>
-      <c r="C39" t="s">
-        <v>316</v>
-      </c>
-      <c r="D39" t="s">
-        <v>317</v>
-      </c>
-      <c r="E39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" t="s">
-        <v>316</v>
-      </c>
-      <c r="G39" t="s">
-        <v>318</v>
-      </c>
-      <c r="H39" t="s">
-        <v>319</v>
-      </c>
-      <c r="I39" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" t="s">
-        <v>320</v>
-      </c>
-      <c r="K39" t="s">
-        <v>321</v>
-      </c>
-      <c r="L39" t="s">
-        <v>322</v>
-      </c>
-      <c r="M39" t="s">
-        <v>18</v>
-      </c>
-      <c r="N39" t="s">
-        <v>18</v>
-      </c>
-      <c r="O39" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C40" t="s">
+        <v>323</v>
+      </c>
+      <c r="D40" t="s">
+        <v>324</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>323</v>
+      </c>
+      <c r="G40" t="s">
+        <v>325</v>
+      </c>
+      <c r="H40" t="s">
+        <v>326</v>
+      </c>
+      <c r="I40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" t="s">
+        <v>327</v>
+      </c>
+      <c r="K40" t="s">
+        <v>328</v>
+      </c>
+      <c r="L40" t="s">
+        <v>50</v>
+      </c>
+      <c r="M40" t="s">
+        <v>18</v>
+      </c>
+      <c r="N40" t="s">
+        <v>18</v>
+      </c>
+      <c r="O40" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>